<commit_message>
raw data to construct the bode plot
</commit_message>
<xml_diff>
--- a/ControlLab/Lab4/raw_data.xlsx
+++ b/ControlLab/Lab4/raw_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Github\Control-Labs\ControlLab\Lab4\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{407C54C4-52A4-47E2-8CD5-FFAE822A402D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A51E0B6-E0C7-426E-94E6-1FBF3097FBCB}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="38280" yWindow="3630" windowWidth="29040" windowHeight="15990" xr2:uid="{C2172214-EF15-48B2-B9ED-15B451D67939}"/>
   </bookViews>
@@ -403,15 +403,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CF292EA4-4FE1-4721-AE3E-D16586974B76}">
-  <dimension ref="A1:I37"/>
+  <dimension ref="A1:O37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K26" sqref="K26"/>
+      <selection activeCell="G31" sqref="G31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -431,7 +431,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>0.5</v>
       </c>
@@ -448,8 +448,18 @@
         <f>D2*-1</f>
         <v>-3</v>
       </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="M2">
+        <v>0.5</v>
+      </c>
+      <c r="N2">
+        <f>C2/B2</f>
+        <v>2.0404040404040402</v>
+      </c>
+      <c r="O2">
+        <v>-3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1</v>
       </c>
@@ -466,8 +476,18 @@
         <f t="shared" ref="I3:I5" si="0">D3*-1</f>
         <v>-2</v>
       </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="M3">
+        <v>1</v>
+      </c>
+      <c r="N3">
+        <f t="shared" ref="N3:N37" si="1">C3/B3</f>
+        <v>2.0408163265306123</v>
+      </c>
+      <c r="O3">
+        <v>-2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>2</v>
       </c>
@@ -484,8 +504,18 @@
         <f t="shared" si="0"/>
         <v>-11</v>
       </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="M4">
+        <v>2</v>
+      </c>
+      <c r="N4">
+        <f t="shared" si="1"/>
+        <v>2.0714285714285712</v>
+      </c>
+      <c r="O4">
+        <v>-11</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>3</v>
       </c>
@@ -502,13 +532,23 @@
         <f t="shared" si="0"/>
         <v>-12</v>
       </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="M5">
+        <v>3</v>
+      </c>
+      <c r="N5">
+        <f t="shared" si="1"/>
+        <v>2.0358056265984654</v>
+      </c>
+      <c r="O5">
+        <v>-12</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>4</v>
       </c>
       <c r="B6">
-        <v>2.91</v>
+        <v>3.91</v>
       </c>
       <c r="C6">
         <v>7.46</v>
@@ -521,8 +561,18 @@
         <f>-A6*G6*10^-3*360</f>
         <v>-23.04</v>
       </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="M6">
+        <v>4</v>
+      </c>
+      <c r="N6">
+        <f t="shared" si="1"/>
+        <v>1.907928388746803</v>
+      </c>
+      <c r="O6">
+        <v>-23.04</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>5</v>
       </c>
@@ -536,11 +586,21 @@
         <v>16</v>
       </c>
       <c r="I7">
-        <f t="shared" ref="I7:I37" si="1">-A7*G7*10^-3*360</f>
+        <f t="shared" ref="I7:I37" si="2">-A7*G7*10^-3*360</f>
         <v>-28.8</v>
       </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="M7">
+        <v>5</v>
+      </c>
+      <c r="N7">
+        <f t="shared" si="1"/>
+        <v>1.9335038363171353</v>
+      </c>
+      <c r="O7">
+        <v>-28.8</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>6</v>
       </c>
@@ -555,11 +615,21 @@
         <v>16</v>
       </c>
       <c r="I8">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>-34.56</v>
       </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="M8">
+        <v>6</v>
+      </c>
+      <c r="N8">
+        <f t="shared" si="1"/>
+        <v>1.8439897698209717</v>
+      </c>
+      <c r="O8">
+        <v>-34.56</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>7</v>
       </c>
@@ -573,11 +643,21 @@
         <v>16</v>
       </c>
       <c r="I9">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>-40.32</v>
       </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="M9">
+        <v>7</v>
+      </c>
+      <c r="N9">
+        <f t="shared" si="1"/>
+        <v>1.7048346055979644</v>
+      </c>
+      <c r="O9">
+        <v>-40.32</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>8</v>
       </c>
@@ -591,11 +671,21 @@
         <v>14.8</v>
       </c>
       <c r="I10">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>-42.624000000000002</v>
       </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="M10">
+        <v>8</v>
+      </c>
+      <c r="N10">
+        <f t="shared" si="1"/>
+        <v>1.6751918158567773</v>
+      </c>
+      <c r="O10">
+        <v>-42.624000000000002</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>9</v>
       </c>
@@ -609,11 +699,21 @@
         <v>12.8</v>
       </c>
       <c r="I11">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>-41.472000000000001</v>
       </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="M11">
+        <v>9</v>
+      </c>
+      <c r="N11">
+        <f t="shared" si="1"/>
+        <v>1.6496163682864451</v>
+      </c>
+      <c r="O11">
+        <v>-41.472000000000001</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>10</v>
       </c>
@@ -627,11 +727,21 @@
         <v>13.6</v>
       </c>
       <c r="I12">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>-48.96</v>
       </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="M12">
+        <v>10</v>
+      </c>
+      <c r="N12">
+        <f t="shared" si="1"/>
+        <v>1.5984654731457799</v>
+      </c>
+      <c r="O12">
+        <v>-48.96</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>11</v>
       </c>
@@ -645,11 +755,21 @@
         <v>13.2</v>
       </c>
       <c r="I13">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>-52.271999999999998</v>
       </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="M13">
+        <v>11</v>
+      </c>
+      <c r="N13">
+        <f t="shared" si="1"/>
+        <v>1.5601023017902811</v>
+      </c>
+      <c r="O13">
+        <v>-52.271999999999998</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>12</v>
       </c>
@@ -663,11 +783,21 @@
         <v>13.2</v>
       </c>
       <c r="I14">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>-57.023999999999994</v>
       </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="M14">
+        <v>12</v>
+      </c>
+      <c r="N14">
+        <f t="shared" si="1"/>
+        <v>1.5217391304347827</v>
+      </c>
+      <c r="O14">
+        <v>-57.023999999999994</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>13</v>
       </c>
@@ -681,11 +811,21 @@
         <v>12.4</v>
       </c>
       <c r="I15">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>-58.032000000000004</v>
       </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="M15">
+        <v>13</v>
+      </c>
+      <c r="N15">
+        <f t="shared" si="1"/>
+        <v>1.4885496183206106</v>
+      </c>
+      <c r="O15">
+        <v>-58.032000000000004</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>14</v>
       </c>
@@ -699,11 +839,21 @@
         <v>12.4</v>
       </c>
       <c r="I16">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>-62.496000000000002</v>
       </c>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="M16">
+        <v>14</v>
+      </c>
+      <c r="N16">
+        <f t="shared" si="1"/>
+        <v>1.3785166240409206</v>
+      </c>
+      <c r="O16">
+        <v>-62.496000000000002</v>
+      </c>
+    </row>
+    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>15</v>
       </c>
@@ -711,17 +861,27 @@
         <v>3.91</v>
       </c>
       <c r="C17">
-        <v>5.44</v>
+        <v>5.2</v>
       </c>
       <c r="G17">
         <v>11.6</v>
       </c>
       <c r="I17">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>-62.640000000000008</v>
       </c>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="M17">
+        <v>15</v>
+      </c>
+      <c r="N17">
+        <f t="shared" si="1"/>
+        <v>1.329923273657289</v>
+      </c>
+      <c r="O17">
+        <v>-62.640000000000008</v>
+      </c>
+    </row>
+    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>16</v>
       </c>
@@ -735,11 +895,21 @@
         <v>11.6</v>
       </c>
       <c r="I18">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>-66.816000000000003</v>
       </c>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="M18">
+        <v>16</v>
+      </c>
+      <c r="N18">
+        <f t="shared" si="1"/>
+        <v>1.289002557544757</v>
+      </c>
+      <c r="O18">
+        <v>-66.816000000000003</v>
+      </c>
+    </row>
+    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>17</v>
       </c>
@@ -753,11 +923,21 @@
         <v>11.2</v>
       </c>
       <c r="I19">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>-68.543999999999997</v>
       </c>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="M19">
+        <v>17</v>
+      </c>
+      <c r="N19">
+        <f t="shared" si="1"/>
+        <v>1.3017902813299231</v>
+      </c>
+      <c r="O19">
+        <v>-68.543999999999997</v>
+      </c>
+    </row>
+    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>18</v>
       </c>
@@ -771,11 +951,21 @@
         <v>10.8</v>
       </c>
       <c r="I20">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>-69.984000000000009</v>
       </c>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="M20">
+        <v>18</v>
+      </c>
+      <c r="N20">
+        <f t="shared" si="1"/>
+        <v>1.2122762148337596</v>
+      </c>
+      <c r="O20">
+        <v>-69.984000000000009</v>
+      </c>
+    </row>
+    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>19</v>
       </c>
@@ -788,12 +978,25 @@
       <c r="D21">
         <v>71</v>
       </c>
+      <c r="G21">
+        <v>10.4</v>
+      </c>
       <c r="I21">
-        <f>D21*-1</f>
-        <v>-71</v>
-      </c>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+        <f t="shared" si="2"/>
+        <v>-71.135999999999996</v>
+      </c>
+      <c r="M21">
+        <v>19</v>
+      </c>
+      <c r="N21">
+        <f t="shared" si="1"/>
+        <v>1.1958762886597938</v>
+      </c>
+      <c r="O21">
+        <v>-71.135999999999996</v>
+      </c>
+    </row>
+    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>20</v>
       </c>
@@ -806,12 +1009,25 @@
       <c r="D22">
         <v>69</v>
       </c>
+      <c r="G22">
+        <v>10.4</v>
+      </c>
       <c r="I22">
-        <f t="shared" ref="I22:I29" si="2">D22*-1</f>
-        <v>-69</v>
-      </c>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+        <f t="shared" si="2"/>
+        <v>-74.88000000000001</v>
+      </c>
+      <c r="M22">
+        <v>20</v>
+      </c>
+      <c r="N22">
+        <f t="shared" si="1"/>
+        <v>1.1829896907216495</v>
+      </c>
+      <c r="O22">
+        <v>-74.88000000000001</v>
+      </c>
+    </row>
+    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>22</v>
       </c>
@@ -824,12 +1040,25 @@
       <c r="D23">
         <v>75</v>
       </c>
+      <c r="G23">
+        <v>10</v>
+      </c>
       <c r="I23">
         <f t="shared" si="2"/>
-        <v>-75</v>
-      </c>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+        <v>-79.2</v>
+      </c>
+      <c r="M23">
+        <v>22</v>
+      </c>
+      <c r="N23">
+        <f t="shared" si="1"/>
+        <v>1.0902061855670104</v>
+      </c>
+      <c r="O23">
+        <v>-79.2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>24</v>
       </c>
@@ -842,12 +1071,25 @@
       <c r="D24">
         <v>75</v>
       </c>
+      <c r="G24">
+        <v>9.6</v>
+      </c>
       <c r="I24">
         <f t="shared" si="2"/>
-        <v>-75</v>
-      </c>
-    </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+        <v>-82.944000000000003</v>
+      </c>
+      <c r="M24">
+        <v>24</v>
+      </c>
+      <c r="N24">
+        <f t="shared" si="1"/>
+        <v>0.99484536082474229</v>
+      </c>
+      <c r="O24">
+        <v>-82.944000000000003</v>
+      </c>
+    </row>
+    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>26</v>
       </c>
@@ -860,12 +1102,25 @@
       <c r="D25">
         <v>82</v>
       </c>
+      <c r="G25">
+        <v>9.6</v>
+      </c>
       <c r="I25">
         <f t="shared" si="2"/>
-        <v>-82</v>
-      </c>
-    </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+        <v>-89.855999999999995</v>
+      </c>
+      <c r="M25">
+        <v>26</v>
+      </c>
+      <c r="N25">
+        <f t="shared" si="1"/>
+        <v>0.94629156010230175</v>
+      </c>
+      <c r="O25">
+        <v>-89.855999999999995</v>
+      </c>
+    </row>
+    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>28</v>
       </c>
@@ -878,12 +1133,25 @@
       <c r="D26">
         <v>84</v>
       </c>
+      <c r="G26">
+        <v>9.1999999999999993</v>
+      </c>
       <c r="I26">
         <f t="shared" si="2"/>
-        <v>-84</v>
-      </c>
-    </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+        <v>-92.736000000000004</v>
+      </c>
+      <c r="M26">
+        <v>28</v>
+      </c>
+      <c r="N26">
+        <f t="shared" si="1"/>
+        <v>0.90463917525773196</v>
+      </c>
+      <c r="O26">
+        <v>-92.736000000000004</v>
+      </c>
+    </row>
+    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>30</v>
       </c>
@@ -896,12 +1164,25 @@
       <c r="D27">
         <v>87</v>
       </c>
+      <c r="G27">
+        <v>8.8000000000000007</v>
+      </c>
       <c r="I27">
         <f t="shared" si="2"/>
-        <v>-87</v>
-      </c>
-    </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+        <v>-95.04</v>
+      </c>
+      <c r="M27">
+        <v>30</v>
+      </c>
+      <c r="N27">
+        <f t="shared" si="1"/>
+        <v>0.84793814432989689</v>
+      </c>
+      <c r="O27">
+        <v>-95.04</v>
+      </c>
+    </row>
+    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>35</v>
       </c>
@@ -914,12 +1195,25 @@
       <c r="D28">
         <v>95</v>
       </c>
+      <c r="G28">
+        <v>8.4</v>
+      </c>
       <c r="I28">
         <f t="shared" si="2"/>
-        <v>-95</v>
-      </c>
-    </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+        <v>-105.83999999999999</v>
+      </c>
+      <c r="M28">
+        <v>35</v>
+      </c>
+      <c r="N28">
+        <f t="shared" si="1"/>
+        <v>0.72680412371134018</v>
+      </c>
+      <c r="O28">
+        <v>-105.83999999999999</v>
+      </c>
+    </row>
+    <row r="29" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>40</v>
       </c>
@@ -932,12 +1226,25 @@
       <c r="D29">
         <v>108</v>
       </c>
+      <c r="G29">
+        <v>7.6</v>
+      </c>
       <c r="I29">
         <f t="shared" si="2"/>
-        <v>-108</v>
-      </c>
-    </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+        <v>-109.44</v>
+      </c>
+      <c r="M29">
+        <v>40</v>
+      </c>
+      <c r="N29">
+        <f t="shared" si="1"/>
+        <v>0.64194373401534521</v>
+      </c>
+      <c r="O29">
+        <v>-109.44</v>
+      </c>
+    </row>
+    <row r="30" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>45</v>
       </c>
@@ -947,15 +1254,28 @@
       <c r="C30">
         <v>2.23</v>
       </c>
+      <c r="D30">
+        <v>116</v>
+      </c>
       <c r="G30">
-        <v>7.6</v>
+        <v>7.2</v>
       </c>
       <c r="I30">
-        <f t="shared" si="1"/>
-        <v>-123.12</v>
-      </c>
-    </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+        <f t="shared" si="2"/>
+        <v>-116.64</v>
+      </c>
+      <c r="M30">
+        <v>45</v>
+      </c>
+      <c r="N30">
+        <f t="shared" si="1"/>
+        <v>0.57474226804123707</v>
+      </c>
+      <c r="O30">
+        <v>-116.64</v>
+      </c>
+    </row>
+    <row r="31" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>50</v>
       </c>
@@ -965,15 +1285,28 @@
       <c r="C31">
         <v>2.09</v>
       </c>
+      <c r="D31">
+        <v>118</v>
+      </c>
       <c r="G31">
         <v>7.2</v>
       </c>
       <c r="I31">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>-129.6</v>
       </c>
-    </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="M31">
+        <v>50</v>
+      </c>
+      <c r="N31">
+        <f t="shared" si="1"/>
+        <v>0.53865979381443296</v>
+      </c>
+      <c r="O31">
+        <v>-129.6</v>
+      </c>
+    </row>
+    <row r="32" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>60</v>
       </c>
@@ -981,17 +1314,30 @@
         <v>3.93</v>
       </c>
       <c r="C32">
-        <v>1.69</v>
+        <v>1.8</v>
+      </c>
+      <c r="D32">
+        <v>128</v>
       </c>
       <c r="G32">
         <v>6.2</v>
       </c>
       <c r="I32">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>-133.91999999999999</v>
       </c>
-    </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="M32">
+        <v>60</v>
+      </c>
+      <c r="N32">
+        <f t="shared" si="1"/>
+        <v>0.4580152671755725</v>
+      </c>
+      <c r="O32">
+        <v>-133.91999999999999</v>
+      </c>
+    </row>
+    <row r="33" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>70</v>
       </c>
@@ -1001,15 +1347,28 @@
       <c r="C33">
         <v>1.49</v>
       </c>
+      <c r="D33">
+        <v>140</v>
+      </c>
       <c r="G33">
         <v>6.2</v>
       </c>
       <c r="I33">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>-156.24</v>
       </c>
-    </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="M33">
+        <v>70</v>
+      </c>
+      <c r="N33">
+        <f t="shared" si="1"/>
+        <v>0.38107416879795397</v>
+      </c>
+      <c r="O33">
+        <v>-156.24</v>
+      </c>
+    </row>
+    <row r="34" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>80</v>
       </c>
@@ -1019,15 +1378,28 @@
       <c r="C34">
         <v>1.3</v>
       </c>
+      <c r="D34">
+        <v>144</v>
+      </c>
       <c r="G34">
         <v>5.76</v>
       </c>
       <c r="I34">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>-165.88800000000001</v>
       </c>
-    </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="M34">
+        <v>80</v>
+      </c>
+      <c r="N34">
+        <f t="shared" si="1"/>
+        <v>0.33078880407124683</v>
+      </c>
+      <c r="O34">
+        <v>-165.88800000000001</v>
+      </c>
+    </row>
+    <row r="35" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>90</v>
       </c>
@@ -1041,11 +1413,21 @@
         <v>5.52</v>
       </c>
       <c r="I35">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>-178.84799999999998</v>
       </c>
-    </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="M35">
+        <v>90</v>
+      </c>
+      <c r="N35">
+        <f t="shared" si="1"/>
+        <v>0.29156010230179025</v>
+      </c>
+      <c r="O35">
+        <v>-178.84799999999998</v>
+      </c>
+    </row>
+    <row r="36" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>100</v>
       </c>
@@ -1059,11 +1441,21 @@
         <v>5.28</v>
       </c>
       <c r="I36">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>-190.08</v>
       </c>
-    </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="M36">
+        <v>100</v>
+      </c>
+      <c r="N36">
+        <f t="shared" si="1"/>
+        <v>0.2608695652173913</v>
+      </c>
+      <c r="O36">
+        <v>-190.08</v>
+      </c>
+    </row>
+    <row r="37" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>110</v>
       </c>
@@ -1077,7 +1469,17 @@
         <v>4.96</v>
       </c>
       <c r="I37">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
+        <v>-196.41600000000003</v>
+      </c>
+      <c r="M37">
+        <v>110</v>
+      </c>
+      <c r="N37">
+        <f t="shared" si="1"/>
+        <v>0.26717557251908397</v>
+      </c>
+      <c r="O37">
         <v>-196.41600000000003</v>
       </c>
     </row>

</xml_diff>